<commit_message>
WIP: Move to modules for TMP Units.
Includes updated scripts for unit generation and fixes.
</commit_message>
<xml_diff>
--- a/modules/tmp_units/generator/Units_Library.xlsx
+++ b/modules/tmp_units/generator/Units_Library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\tmp-units\generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\vanir\modules\tmp_units\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F1816E-621B-4D1A-9CF6-52807FB3F08D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5FE96D-9122-4B48-A0DC-E1051F44F48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="12667" windowHeight="13680" firstSheet="3" activeTab="5" xr2:uid="{FE6D38CB-547E-4C55-8C75-9181182D2542}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{FE6D38CB-547E-4C55-8C75-9181182D2542}"/>
   </bookViews>
   <sheets>
     <sheet name="SI_Prefixes" sheetId="4" r:id="rId1"/>
@@ -578,9 +578,6 @@
     <t>heat_capacity</t>
   </si>
   <si>
-    <t>specfic_heat_capacity</t>
-  </si>
-  <si>
     <t>surface_charge_density</t>
   </si>
   <si>
@@ -1653,6 +1650,9 @@
   </si>
   <si>
     <t>proton_mass</t>
+  </si>
+  <si>
+    <t>specific_heat_capacity</t>
   </si>
 </sst>
 </file>
@@ -1724,10 +1724,10 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000000E+00"/>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <numFmt numFmtId="165" formatCode="0.00000000E+00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000000E+00"/>
@@ -1821,8 +1821,8 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{C9B4BB3B-D4F9-4DC3-B9F2-7AD3A9C89B12}" name="Name"/>
     <tableColumn id="2" xr3:uid="{5F19C499-9802-478A-826B-E0A2F082B2B0}" name="Symbol"/>
-    <tableColumn id="3" xr3:uid="{9DB65FF3-ED6F-4C92-AB60-8BDF28AE4D56}" name="Value" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{3EF1A5B6-F4E6-42B7-8B6E-13986C9EF6FE}" name="Units" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{9DB65FF3-ED6F-4C92-AB60-8BDF28AE4D56}" name="Value" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{3EF1A5B6-F4E6-42B7-8B6E-13986C9EF6FE}" name="Units" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{B65D9669-7FC0-44E7-AE6C-9415301E3797}" name="Impl Num"/>
     <tableColumn id="7" xr3:uid="{441DE776-25FC-4A04-9252-9923D50A465D}" name="Impl Den"/>
     <tableColumn id="8" xr3:uid="{4C90A15A-2C71-487A-BED6-27724CE9FF54}" name="Desc"/>
@@ -2134,15 +2134,15 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.46875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.76171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>125</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>9.9999999999999998E+23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>1E+21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>131</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>1E+18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>134</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>1000000000000000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>136</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>1000000000000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>137</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>139</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>0</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>147</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>149</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>151</v>
       </c>
@@ -2360,12 +2360,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>152</v>
       </c>
       <c r="B16" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C16">
         <v>-6</v>
@@ -2375,7 +2375,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>153</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>155</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>9.9999999999999998E-13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>157</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>1.0000000000000001E-15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>159</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>1.0000000000000001E-18</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>161</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>9.9999999999999991E-22</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>163</v>
       </c>
@@ -2484,17 +2484,17 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.46875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.3515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.52734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.234375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.41015625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.46875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E1" t="s">
         <v>7</v>
@@ -2517,12 +2517,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C2" t="s">
         <v>38</v>
@@ -2531,13 +2531,13 @@
         <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2551,10 +2551,10 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -2568,13 +2568,13 @@
         <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F4" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2588,13 +2588,13 @@
         <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -2608,13 +2608,13 @@
         <v>74</v>
       </c>
       <c r="E6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F6" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -2628,10 +2628,10 @@
         <v>66</v>
       </c>
       <c r="E7" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -2645,30 +2645,30 @@
         <v>167</v>
       </c>
       <c r="E8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>417</v>
+      </c>
+      <c r="B9" t="s">
         <v>418</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>419</v>
       </c>
-      <c r="C9" t="s">
-        <v>420</v>
-      </c>
       <c r="D9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F9" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -2682,13 +2682,13 @@
         <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -2702,13 +2702,13 @@
         <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F11" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -2722,10 +2722,10 @@
         <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -2739,13 +2739,13 @@
         <v>77</v>
       </c>
       <c r="E13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -2759,13 +2759,13 @@
         <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F14" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -2779,10 +2779,10 @@
         <v>165</v>
       </c>
       <c r="E15" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -2796,10 +2796,10 @@
         <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -2813,10 +2813,10 @@
         <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -2830,13 +2830,13 @@
         <v>57</v>
       </c>
       <c r="E18" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F18" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -2850,30 +2850,30 @@
         <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -2887,10 +2887,10 @@
         <v>86</v>
       </c>
       <c r="E21" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -2904,18 +2904,18 @@
         <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F22" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C23" t="s">
         <v>36</v>
@@ -2924,13 +2924,13 @@
         <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F23" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>70</v>
       </c>
@@ -2958,16 +2958,16 @@
         <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E25" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F25" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -2981,10 +2981,10 @@
         <v>83</v>
       </c>
       <c r="E26" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>166</v>
       </c>
       <c r="E27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3018,15 +3018,15 @@
       <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.64453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.3515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.3515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.8203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -3055,7 +3055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -3075,13 +3075,13 @@
         <v>171</v>
       </c>
       <c r="G2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3095,44 +3095,44 @@
         <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G4" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B5" t="s">
         <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E5" t="s">
         <v>174</v>
@@ -3141,15 +3141,15 @@
         <v>168</v>
       </c>
       <c r="G5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s">
         <v>95</v>
@@ -3158,7 +3158,7 @@
         <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E6" t="s">
         <v>168</v>
@@ -3167,15 +3167,15 @@
         <v>171</v>
       </c>
       <c r="G6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B7" t="s">
         <v>88</v>
@@ -3184,7 +3184,7 @@
         <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E7" t="s">
         <v>169</v>
@@ -3193,24 +3193,24 @@
         <v>171</v>
       </c>
       <c r="G7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B8" t="s">
         <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E8" t="s">
         <v>169</v>
@@ -3219,24 +3219,24 @@
         <v>172</v>
       </c>
       <c r="G8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H8" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>481</v>
+      </c>
+      <c r="B9" t="s">
         <v>482</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>483</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>484</v>
-      </c>
-      <c r="D9" t="s">
-        <v>485</v>
       </c>
       <c r="E9" t="s">
         <v>170</v>
@@ -3245,24 +3245,24 @@
         <v>172</v>
       </c>
       <c r="G9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>278</v>
+      </c>
+      <c r="B10" t="s">
         <v>279</v>
       </c>
-      <c r="B10" t="s">
-        <v>280</v>
-      </c>
       <c r="C10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E10" t="s">
         <v>170</v>
@@ -3271,124 +3271,124 @@
         <v>173</v>
       </c>
       <c r="G10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H10" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>354</v>
+      </c>
+      <c r="B11" t="s">
+        <v>277</v>
+      </c>
+      <c r="C11" t="s">
+        <v>357</v>
+      </c>
+      <c r="D11" t="s">
+        <v>351</v>
+      </c>
+      <c r="E11" t="s">
+        <v>194</v>
+      </c>
+      <c r="F11" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>355</v>
       </c>
-      <c r="B11" t="s">
-        <v>278</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B12" t="s">
+        <v>273</v>
+      </c>
+      <c r="C12" t="s">
         <v>358</v>
       </c>
-      <c r="D11" t="s">
-        <v>352</v>
-      </c>
-      <c r="E11" t="s">
-        <v>195</v>
-      </c>
-      <c r="F11" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A12" t="s">
+      <c r="D12" t="s">
+        <v>349</v>
+      </c>
+      <c r="F12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>356</v>
-      </c>
-      <c r="B12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C12" t="s">
-        <v>359</v>
-      </c>
-      <c r="D12" t="s">
-        <v>350</v>
-      </c>
-      <c r="F12" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A13" t="s">
-        <v>357</v>
       </c>
       <c r="B13" t="s">
         <v>116</v>
       </c>
       <c r="C13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>467</v>
+      </c>
+      <c r="B14" t="s">
         <v>468</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>469</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>470</v>
       </c>
-      <c r="D14" t="s">
-        <v>471</v>
-      </c>
       <c r="E14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F14" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B15" t="s">
         <v>98</v>
       </c>
       <c r="C15" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F15" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B16" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D16" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E16" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -3400,21 +3400,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD48556E-ABA2-4F61-AE13-AC43D331C84E}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:XFD57"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.29296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.64453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.234375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.41015625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.46875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E1" t="s">
         <v>7</v>
@@ -3437,9 +3437,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B2" t="s">
         <v>110</v>
@@ -3448,78 +3448,78 @@
         <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>447</v>
+      </c>
+      <c r="B4" t="s">
         <v>448</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>449</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>450</v>
       </c>
-      <c r="D4" t="s">
-        <v>451</v>
-      </c>
       <c r="E4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B5" t="s">
         <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
         <v>90</v>
@@ -3528,175 +3528,175 @@
         <v>91</v>
       </c>
       <c r="D6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B8" t="s">
         <v>115</v>
       </c>
       <c r="C8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D8" t="s">
+        <v>341</v>
+      </c>
+      <c r="E8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>248</v>
+      </c>
+      <c r="B9" t="s">
+        <v>249</v>
+      </c>
+      <c r="C9" t="s">
+        <v>399</v>
+      </c>
+      <c r="D9" t="s">
         <v>342</v>
       </c>
-      <c r="E8" t="s">
-        <v>185</v>
-      </c>
-      <c r="F8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A9" t="s">
-        <v>249</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="E9" t="s">
+        <v>183</v>
+      </c>
+      <c r="F9" t="s">
         <v>250</v>
       </c>
-      <c r="C9" t="s">
-        <v>400</v>
-      </c>
-      <c r="D9" t="s">
-        <v>343</v>
-      </c>
-      <c r="E9" t="s">
-        <v>184</v>
-      </c>
-      <c r="F9" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B10" t="s">
         <v>123</v>
       </c>
       <c r="C10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F10" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B11" t="s">
         <v>120</v>
       </c>
       <c r="C11" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F11" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B12" t="s">
         <v>117</v>
       </c>
       <c r="C12" t="s">
+        <v>501</v>
+      </c>
+      <c r="D12" t="s">
         <v>502</v>
       </c>
-      <c r="D12" t="s">
-        <v>503</v>
-      </c>
       <c r="E12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B13" t="s">
         <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F13" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B14" t="s">
         <v>101</v>
       </c>
       <c r="C14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B15" t="s">
         <v>99</v>
@@ -3705,78 +3705,78 @@
         <v>100</v>
       </c>
       <c r="D15" t="s">
+        <v>303</v>
+      </c>
+      <c r="E15" t="s">
+        <v>511</v>
+      </c>
+      <c r="F15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>421</v>
+      </c>
+      <c r="B16" t="s">
+        <v>422</v>
+      </c>
+      <c r="C16" t="s">
+        <v>423</v>
+      </c>
+      <c r="D16" t="s">
+        <v>424</v>
+      </c>
+      <c r="E16" t="s">
+        <v>512</v>
+      </c>
+      <c r="F16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>251</v>
+      </c>
+      <c r="B17" t="s">
+        <v>252</v>
+      </c>
+      <c r="C17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D17" t="s">
         <v>304</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E17" t="s">
+        <v>202</v>
+      </c>
+      <c r="F17" t="s">
         <v>512</v>
       </c>
-      <c r="F15" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A16" t="s">
-        <v>422</v>
-      </c>
-      <c r="B16" t="s">
-        <v>423</v>
-      </c>
-      <c r="C16" t="s">
-        <v>424</v>
-      </c>
-      <c r="D16" t="s">
-        <v>425</v>
-      </c>
-      <c r="E16" t="s">
-        <v>513</v>
-      </c>
-      <c r="F16" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A17" t="s">
-        <v>252</v>
-      </c>
-      <c r="B17" t="s">
-        <v>253</v>
-      </c>
-      <c r="C17" t="s">
-        <v>254</v>
-      </c>
-      <c r="D17" t="s">
-        <v>305</v>
-      </c>
-      <c r="E17" t="s">
-        <v>203</v>
-      </c>
-      <c r="F17" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>463</v>
+      </c>
+      <c r="B18" t="s">
         <v>464</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>465</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>466</v>
       </c>
-      <c r="D18" t="s">
-        <v>467</v>
-      </c>
       <c r="E18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F18" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B19" t="s">
         <v>108</v>
@@ -3785,35 +3785,35 @@
         <v>109</v>
       </c>
       <c r="D19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F19" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>434</v>
+      </c>
+      <c r="B20" t="s">
         <v>435</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>436</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>437</v>
       </c>
-      <c r="D20" t="s">
-        <v>438</v>
-      </c>
       <c r="F20" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B21" t="s">
         <v>178</v>
@@ -3822,132 +3822,132 @@
         <v>94</v>
       </c>
       <c r="D21" t="s">
+        <v>306</v>
+      </c>
+      <c r="E21" t="s">
+        <v>506</v>
+      </c>
+      <c r="F21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>425</v>
+      </c>
+      <c r="B22" t="s">
+        <v>426</v>
+      </c>
+      <c r="C22" t="s">
+        <v>430</v>
+      </c>
+      <c r="D22" t="s">
+        <v>427</v>
+      </c>
+      <c r="E22" t="s">
+        <v>182</v>
+      </c>
+      <c r="F22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>256</v>
+      </c>
+      <c r="B23" t="s">
+        <v>257</v>
+      </c>
+      <c r="C23" t="s">
+        <v>258</v>
+      </c>
+      <c r="D23" t="s">
         <v>307</v>
       </c>
-      <c r="E21" t="s">
-        <v>507</v>
-      </c>
-      <c r="F21" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A22" t="s">
-        <v>426</v>
-      </c>
-      <c r="B22" t="s">
-        <v>427</v>
-      </c>
-      <c r="C22" t="s">
-        <v>431</v>
-      </c>
-      <c r="D22" t="s">
-        <v>428</v>
-      </c>
-      <c r="E22" t="s">
-        <v>183</v>
-      </c>
-      <c r="F22" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A23" t="s">
-        <v>257</v>
-      </c>
-      <c r="B23" t="s">
-        <v>258</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
+        <v>198</v>
+      </c>
+      <c r="F23" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>269</v>
+      </c>
+      <c r="B24" t="s">
+        <v>270</v>
+      </c>
+      <c r="C24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D24" t="s">
+        <v>308</v>
+      </c>
+      <c r="E24" t="s">
+        <v>272</v>
+      </c>
+      <c r="F24" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>263</v>
+      </c>
+      <c r="B25" t="s">
+        <v>264</v>
+      </c>
+      <c r="C25" t="s">
+        <v>265</v>
+      </c>
+      <c r="D25" t="s">
+        <v>323</v>
+      </c>
+      <c r="E25" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>267</v>
+      </c>
+      <c r="B26" t="s">
+        <v>268</v>
+      </c>
+      <c r="C26" t="s">
+        <v>409</v>
+      </c>
+      <c r="D26" t="s">
+        <v>338</v>
+      </c>
+      <c r="E26" t="s">
+        <v>266</v>
+      </c>
+      <c r="F26" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>259</v>
       </c>
-      <c r="D23" t="s">
-        <v>308</v>
-      </c>
-      <c r="E23" t="s">
-        <v>199</v>
-      </c>
-      <c r="F23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A24" t="s">
-        <v>270</v>
-      </c>
-      <c r="B24" t="s">
-        <v>271</v>
-      </c>
-      <c r="C24" t="s">
-        <v>272</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B27" t="s">
+        <v>260</v>
+      </c>
+      <c r="C27" t="s">
+        <v>261</v>
+      </c>
+      <c r="D27" t="s">
         <v>309</v>
       </c>
-      <c r="E24" t="s">
-        <v>273</v>
-      </c>
-      <c r="F24" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A25" t="s">
-        <v>264</v>
-      </c>
-      <c r="B25" t="s">
-        <v>265</v>
-      </c>
-      <c r="C25" t="s">
-        <v>266</v>
-      </c>
-      <c r="D25" t="s">
-        <v>324</v>
-      </c>
-      <c r="E25" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A26" t="s">
-        <v>268</v>
-      </c>
-      <c r="B26" t="s">
-        <v>269</v>
-      </c>
-      <c r="C26" t="s">
-        <v>410</v>
-      </c>
-      <c r="D26" t="s">
-        <v>339</v>
-      </c>
-      <c r="E26" t="s">
-        <v>267</v>
-      </c>
-      <c r="F26" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A27" t="s">
-        <v>260</v>
-      </c>
-      <c r="B27" t="s">
-        <v>261</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>262</v>
       </c>
-      <c r="D27" t="s">
-        <v>310</v>
-      </c>
-      <c r="E27" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B28" t="s">
         <v>121</v>
@@ -3956,138 +3956,138 @@
         <v>122</v>
       </c>
       <c r="D28" t="s">
+        <v>310</v>
+      </c>
+      <c r="E28" t="s">
+        <v>185</v>
+      </c>
+      <c r="F28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>280</v>
+      </c>
+      <c r="B29" t="s">
+        <v>281</v>
+      </c>
+      <c r="C29" t="s">
+        <v>282</v>
+      </c>
+      <c r="D29" t="s">
+        <v>324</v>
+      </c>
+      <c r="E29" t="s">
+        <v>512</v>
+      </c>
+      <c r="F29" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>285</v>
+      </c>
+      <c r="B30" t="s">
+        <v>286</v>
+      </c>
+      <c r="C30" t="s">
+        <v>287</v>
+      </c>
+      <c r="D30" t="s">
+        <v>325</v>
+      </c>
+      <c r="E30" t="s">
+        <v>511</v>
+      </c>
+      <c r="F30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>291</v>
+      </c>
+      <c r="B31" t="s">
+        <v>292</v>
+      </c>
+      <c r="C31" t="s">
+        <v>293</v>
+      </c>
+      <c r="D31" t="s">
         <v>311</v>
       </c>
-      <c r="E28" t="s">
-        <v>186</v>
-      </c>
-      <c r="F28" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A29" t="s">
-        <v>281</v>
-      </c>
-      <c r="B29" t="s">
-        <v>282</v>
-      </c>
-      <c r="C29" t="s">
-        <v>283</v>
-      </c>
-      <c r="D29" t="s">
-        <v>325</v>
-      </c>
-      <c r="E29" t="s">
-        <v>513</v>
-      </c>
-      <c r="F29" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A30" t="s">
-        <v>286</v>
-      </c>
-      <c r="B30" t="s">
-        <v>287</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="E31" t="s">
+        <v>194</v>
+      </c>
+      <c r="F31" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>288</v>
       </c>
-      <c r="D30" t="s">
+      <c r="B32" t="s">
+        <v>289</v>
+      </c>
+      <c r="C32" t="s">
+        <v>290</v>
+      </c>
+      <c r="D32" t="s">
         <v>326</v>
       </c>
-      <c r="E30" t="s">
-        <v>512</v>
-      </c>
-      <c r="F30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A31" t="s">
-        <v>292</v>
-      </c>
-      <c r="B31" t="s">
-        <v>293</v>
-      </c>
-      <c r="C31" t="s">
-        <v>294</v>
-      </c>
-      <c r="D31" t="s">
-        <v>312</v>
-      </c>
-      <c r="E31" t="s">
-        <v>195</v>
-      </c>
-      <c r="F31" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A32" t="s">
-        <v>289</v>
-      </c>
-      <c r="B32" t="s">
-        <v>290</v>
-      </c>
-      <c r="C32" t="s">
-        <v>291</v>
-      </c>
-      <c r="D32" t="s">
-        <v>327</v>
-      </c>
       <c r="E32" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F32" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>295</v>
+      </c>
+      <c r="B33" t="s">
+        <v>246</v>
+      </c>
+      <c r="C33" t="s">
         <v>296</v>
       </c>
-      <c r="B33" t="s">
-        <v>247</v>
-      </c>
-      <c r="C33" t="s">
-        <v>297</v>
-      </c>
       <c r="D33" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F33" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>241</v>
+      </c>
+      <c r="B34" t="s">
         <v>242</v>
       </c>
-      <c r="B34" t="s">
-        <v>243</v>
-      </c>
       <c r="C34" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D34" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F34" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B35" t="s">
         <v>106</v>
@@ -4096,115 +4096,115 @@
         <v>107</v>
       </c>
       <c r="D35" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E35" t="s">
+        <v>506</v>
+      </c>
+      <c r="F35" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>231</v>
+      </c>
+      <c r="B36" t="s">
+        <v>180</v>
+      </c>
+      <c r="C36" t="s">
+        <v>284</v>
+      </c>
+      <c r="D36" t="s">
+        <v>327</v>
+      </c>
+      <c r="E36" t="s">
+        <v>506</v>
+      </c>
+      <c r="F36" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>505</v>
+      </c>
+      <c r="B37" t="s">
+        <v>247</v>
+      </c>
+      <c r="C37" t="s">
         <v>507</v>
       </c>
-      <c r="F35" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A36" t="s">
-        <v>232</v>
-      </c>
-      <c r="B36" t="s">
-        <v>181</v>
-      </c>
-      <c r="C36" t="s">
-        <v>285</v>
-      </c>
-      <c r="D36" t="s">
-        <v>328</v>
-      </c>
-      <c r="E36" t="s">
-        <v>507</v>
-      </c>
-      <c r="F36" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A37" t="s">
+      <c r="D37" t="s">
+        <v>352</v>
+      </c>
+      <c r="E37" t="s">
+        <v>238</v>
+      </c>
+      <c r="F37" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>239</v>
+      </c>
+      <c r="B38" t="s">
+        <v>240</v>
+      </c>
+      <c r="C38" t="s">
+        <v>398</v>
+      </c>
+      <c r="D38" t="s">
+        <v>346</v>
+      </c>
+      <c r="E38" t="s">
+        <v>183</v>
+      </c>
+      <c r="F38" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>503</v>
+      </c>
+      <c r="B39" t="s">
+        <v>475</v>
+      </c>
+      <c r="C39" t="s">
+        <v>509</v>
+      </c>
+      <c r="D39" t="s">
+        <v>476</v>
+      </c>
+      <c r="E39" t="s">
         <v>506</v>
       </c>
-      <c r="B37" t="s">
-        <v>248</v>
-      </c>
-      <c r="C37" t="s">
-        <v>508</v>
-      </c>
-      <c r="D37" t="s">
-        <v>353</v>
-      </c>
-      <c r="E37" t="s">
-        <v>239</v>
-      </c>
-      <c r="F37" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A38" t="s">
-        <v>240</v>
-      </c>
-      <c r="B38" t="s">
-        <v>241</v>
-      </c>
-      <c r="C38" t="s">
-        <v>399</v>
-      </c>
-      <c r="D38" t="s">
-        <v>347</v>
-      </c>
-      <c r="E38" t="s">
-        <v>184</v>
-      </c>
-      <c r="F38" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A39" t="s">
-        <v>504</v>
-      </c>
-      <c r="B39" t="s">
-        <v>476</v>
-      </c>
-      <c r="C39" t="s">
-        <v>510</v>
-      </c>
-      <c r="D39" t="s">
-        <v>477</v>
-      </c>
-      <c r="E39" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>438</v>
+      </c>
+      <c r="B40" t="s">
         <v>439</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>440</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>441</v>
       </c>
-      <c r="D40" t="s">
-        <v>442</v>
-      </c>
       <c r="E40" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F40" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B41" t="s">
         <v>104</v>
@@ -4213,18 +4213,18 @@
         <v>105</v>
       </c>
       <c r="D41" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E41" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F41" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B42" t="s">
         <v>102</v>
@@ -4233,58 +4233,58 @@
         <v>103</v>
       </c>
       <c r="D42" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E42" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F42" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B43" t="s">
         <v>114</v>
       </c>
       <c r="C43" t="s">
+        <v>452</v>
+      </c>
+      <c r="D43" t="s">
         <v>453</v>
       </c>
-      <c r="D43" t="s">
-        <v>454</v>
-      </c>
       <c r="E43" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F43" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>471</v>
+      </c>
+      <c r="B44" t="s">
         <v>472</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>473</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>474</v>
       </c>
-      <c r="D44" t="s">
-        <v>475</v>
-      </c>
       <c r="E44" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F44" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B45" t="s">
         <v>112</v>
@@ -4293,290 +4293,290 @@
         <v>113</v>
       </c>
       <c r="D45" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E45" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F45" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>254</v>
+      </c>
+      <c r="B46" t="s">
         <v>255</v>
       </c>
-      <c r="B46" t="s">
-        <v>256</v>
-      </c>
       <c r="C46" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D46" t="s">
+        <v>329</v>
+      </c>
+      <c r="E46" t="s">
+        <v>512</v>
+      </c>
+      <c r="F46" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>428</v>
+      </c>
+      <c r="B47" t="s">
+        <v>429</v>
+      </c>
+      <c r="C47" t="s">
+        <v>431</v>
+      </c>
+      <c r="D47" t="s">
+        <v>432</v>
+      </c>
+      <c r="E47" t="s">
+        <v>182</v>
+      </c>
+      <c r="F47" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>212</v>
+      </c>
+      <c r="B48" t="s">
+        <v>537</v>
+      </c>
+      <c r="C48" t="s">
+        <v>297</v>
+      </c>
+      <c r="D48" t="s">
         <v>330</v>
       </c>
-      <c r="E46" t="s">
-        <v>513</v>
-      </c>
-      <c r="F46" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A47" t="s">
-        <v>429</v>
-      </c>
-      <c r="B47" t="s">
-        <v>430</v>
-      </c>
-      <c r="C47" t="s">
-        <v>432</v>
-      </c>
-      <c r="D47" t="s">
-        <v>433</v>
-      </c>
-      <c r="E47" t="s">
-        <v>183</v>
-      </c>
-      <c r="F47" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A48" t="s">
-        <v>213</v>
-      </c>
-      <c r="B48" t="s">
-        <v>179</v>
-      </c>
-      <c r="C48" t="s">
-        <v>298</v>
-      </c>
-      <c r="D48" t="s">
-        <v>331</v>
-      </c>
       <c r="E48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F48" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.5">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>477</v>
+      </c>
+      <c r="B49" t="s">
         <v>478</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>479</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>480</v>
       </c>
-      <c r="D49" t="s">
-        <v>481</v>
-      </c>
       <c r="E49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F49" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.5">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B50" t="s">
         <v>119</v>
       </c>
       <c r="C50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D50" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E50" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F50" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>459</v>
+      </c>
+      <c r="B51" t="s">
         <v>460</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>461</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>462</v>
       </c>
-      <c r="D51" t="s">
-        <v>463</v>
-      </c>
       <c r="E51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F51" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.5">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>454</v>
+      </c>
+      <c r="B52" t="s">
         <v>455</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>456</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>457</v>
       </c>
-      <c r="D52" t="s">
-        <v>458</v>
-      </c>
       <c r="E52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F52" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.5">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C53" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D53" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E53" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F53" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.5">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B54" t="s">
         <v>118</v>
       </c>
       <c r="C54" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D54" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E54" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F54" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.5">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>274</v>
+      </c>
+      <c r="B55" t="s">
         <v>275</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>276</v>
       </c>
-      <c r="C55" t="s">
-        <v>277</v>
-      </c>
       <c r="D55" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E55" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F55" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.5">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B56" t="s">
         <v>97</v>
       </c>
       <c r="C56" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D56" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E56" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F56" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.5">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B57" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C57" t="s">
         <v>30</v>
       </c>
       <c r="D57" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E57" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F57" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.5">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B58" t="s">
         <v>28</v>
       </c>
       <c r="C58" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D58" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E58" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.5">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>443</v>
+      </c>
+      <c r="B59" t="s">
         <v>444</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>445</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>446</v>
       </c>
-      <c r="D59" t="s">
-        <v>447</v>
-      </c>
       <c r="E59" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F59" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4596,38 +4596,38 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.17578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.64453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.87890625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B1" t="s">
         <v>364</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>365</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>367</v>
-      </c>
       <c r="B2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C2" s="3">
         <v>4046.873</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -4637,9 +4637,9 @@
         <v>1E-10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -4648,9 +4648,9 @@
         <v>149597900000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -4659,9 +4659,9 @@
         <v>0.30480000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -4671,9 +4671,9 @@
         <v>2.5399999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -4682,9 +4682,9 @@
         <v>1609.3440000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -4693,9 +4693,9 @@
         <v>1852</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -4704,9 +4704,9 @@
         <v>3085.6779999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -4715,9 +4715,9 @@
         <v>0.91439999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B11" t="s">
         <v>75</v>
@@ -4726,53 +4726,53 @@
         <v>10.763909999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C12" s="3">
         <v>1550.0029999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C13" s="3">
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C14" s="3">
         <v>9.8066499999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C15" s="3">
         <v>1.355818</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
@@ -4781,9 +4781,9 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
@@ -4792,9 +4792,9 @@
         <v>133.32239999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B18" t="s">
         <v>46</v>
@@ -4803,20 +4803,20 @@
         <v>37000000000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C19" s="3">
         <v>2.5799999999999998E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
@@ -4825,9 +4825,9 @@
         <v>86400</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
@@ -4836,9 +4836,9 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
@@ -4847,75 +4847,75 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C23" s="3">
         <v>0.30480000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C24" s="3">
         <v>3.5239069999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C25" s="3">
         <v>2.3658819999999999E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>389</v>
+      </c>
+      <c r="B26" t="s">
         <v>390</v>
-      </c>
-      <c r="B26" t="s">
-        <v>391</v>
       </c>
       <c r="C26" s="3">
         <v>0.2365882</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C27" s="3">
         <v>9.9999999999999997E-29</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C28" s="3">
         <v>2.9573529999999999E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B29" t="s">
         <v>42</v>
@@ -4937,21 +4937,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C719113B-86D8-499C-B845-F8D8444D585D}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5859375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.17578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.29296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1171875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -4962,7 +4962,7 @@
         <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E1" t="s">
         <v>7</v>
@@ -4974,67 +4974,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B2" t="s">
         <v>493</v>
-      </c>
-      <c r="B2" t="s">
-        <v>494</v>
       </c>
       <c r="C2" s="6">
         <v>9.8066499999999994</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>485</v>
+      </c>
+      <c r="B4" t="s">
         <v>486</v>
-      </c>
-      <c r="B4" t="s">
-        <v>487</v>
       </c>
       <c r="C4" s="5">
         <v>6.0221407599999999E+23</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F4" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B7" t="s">
         <v>142</v>
@@ -5046,19 +5046,19 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>489</v>
+      </c>
+      <c r="B9" t="s">
         <v>490</v>
-      </c>
-      <c r="B9" t="s">
-        <v>491</v>
       </c>
       <c r="C9" s="5">
         <v>1.6021766339999999E-19</v>
@@ -5067,12 +5067,12 @@
         <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B10" t="s">
         <v>69</v>
@@ -5081,67 +5081,67 @@
         <v>96485.332120000006</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F10" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B18" t="s">
         <v>144</v>
@@ -5150,33 +5150,33 @@
         <v>6.6260701499999998E-34</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B22" t="s">
         <v>150</v>
@@ -5188,43 +5188,43 @@
         <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F22" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>494</v>
+      </c>
+      <c r="B23" t="s">
         <v>495</v>
-      </c>
-      <c r="B23" t="s">
-        <v>496</v>
       </c>
       <c r="C23" s="5">
         <v>101325</v>
       </c>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C24" s="5">
         <v>5.6703744189999999E-8</v>
       </c>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="4"/>
@@ -5246,7 +5246,7 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>